<commit_message>
feat: add basic order cancellation logic
</commit_message>
<xml_diff>
--- a/test_data/ride_hailing/example_geographic.xlsx
+++ b/test_data/ride_hailing/example_geographic.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="849">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -2567,6 +2567,9 @@
   </si>
   <si>
     <t xml:space="preserve">seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">order_cancellation_threshold</t>
   </si>
 </sst>
 </file>
@@ -2576,7 +2579,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2611,6 +2614,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2655,7 +2664,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2681,6 +2690,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -12504,16 +12517,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12537,6 +12551,9 @@
       </c>
       <c r="G1" s="3" t="s">
         <v>847</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>848</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat: add fixed incomplete order penalty to reward calculation
</commit_message>
<xml_diff>
--- a/test_data/ride_hailing/example_geographic.xlsx
+++ b/test_data/ride_hailing/example_geographic.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="850">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -2570,6 +2570,9 @@
   </si>
   <si>
     <t xml:space="preserve">order_cancellation_threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incomplete_ride_penalty</t>
   </si>
 </sst>
 </file>
@@ -2579,7 +2582,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2614,12 +2617,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2664,7 +2661,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2690,10 +2687,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -12517,17 +12510,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="22.95"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12552,8 +12546,11 @@
       <c r="G1" s="3" t="s">
         <v>847</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>848</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>849</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12577,6 +12574,9 @@
       </c>
       <c r="G2" s="5" t="n">
         <v>42</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>1439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>